<commit_message>
added b-spline control grid variables
</commit_message>
<xml_diff>
--- a/REG_structure_def.xlsx
+++ b/REG_structure_def.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
   <si>
     <t xml:space="preserve">REG structure definition</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">refIdx</t>
   </si>
   <si>
-    <t xml:space="preserve">int_32</t>
+    <t xml:space="preserve">int32</t>
   </si>
   <si>
     <t xml:space="preserve">Reference image index (index of image in the img array to be used as a reference)</t>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">img[i].ROI</t>
   </si>
   <si>
-    <t xml:space="preserve">1x6 int_32</t>
+    <t xml:space="preserve">1x6 int32</t>
   </si>
   <si>
     <t xml:space="preserve">[1,Nx,1,Ny,1,Nz]</t>
@@ -184,7 +184,7 @@
     <t xml:space="preserve">Deformation field. A displacement in x,y,z direction for each voxel</t>
   </si>
   <si>
-    <t xml:space="preserve">Predefined OPTIONAL fields,rescribing relation to the reference image:</t>
+    <t xml:space="preserve">Predefined OPTIONAL fields, describing image SIMILARITY relation to the reference image:</t>
   </si>
   <si>
     <t xml:space="preserve">img[i].H</t>
@@ -220,7 +220,85 @@
     <t xml:space="preserve">img[i].simWeight</t>
   </si>
   <si>
-    <t xml:space="preserve">number of voxels involved in last similarity estimation</t>
+    <t xml:space="preserve">number of voxels involved in the latest similarity estimation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fields for spline deformation grid of control points (implemented in +cg subfolder=cg package:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img[i].cg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Struct as detailed below:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure defining control points grid defining (non-rigid) transformation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ncx,ncy,ncz, np=3] single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matrix of control points displacements of size ncx*ncy*ncz*np; np=number of parameters=3 for displacements in  [x,y,z] direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x3 int32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb of voxels between two control points(vector [stepx, stepy, stepz])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">margin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">margin beyond the image defined in nb of voxels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enumerated (Int32)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enum: 1-3 = bspline order 1-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kernel3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single [nkx,nky,nkz] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the 3D kernel (when the same is used for all of the parameters)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kernelx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single [nkx] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kernely</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single [nky] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kernelz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single [nkz] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kernels{np}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ single [nkx,nky,nkz] }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D kernel (s) – multiple if they differ for different parameters; np – number of parameters</t>
   </si>
 </sst>
 </file>
@@ -230,7 +308,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -266,6 +344,18 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -322,7 +412,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -365,6 +455,26 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -444,10 +554,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -747,6 +857,117 @@
         <v>66</v>
       </c>
     </row>
+    <row r="29" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Updates. The latest focused to point based evaluation
</commit_message>
<xml_diff>
--- a/REG_structure_def.xlsx
+++ b/REG_structure_def.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="97">
   <si>
     <t xml:space="preserve">REG structure definition</t>
   </si>
@@ -221,6 +221,18 @@
   </si>
   <si>
     <t xml:space="preserve">number of voxels involved in the latest similarity estimation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Control points </t>
+  </si>
+  <si>
+    <t xml:space="preserve">segPtPx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[np, 3] double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Control points in image coordinates with 0-based indexing. (Note that Matlab default is 1-based indexing!)</t>
   </si>
   <si>
     <t xml:space="preserve">fields for spline deformation grid of control points (implemented in +cg subfolder=cg package:</t>
@@ -308,7 +320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -351,11 +363,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -412,7 +419,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -473,18 +480,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -550,24 +553,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="65.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,65 +859,61 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="s">
+    <row r="28" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="13"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14" t="s">
+      <c r="D28" s="12"/>
+      <c r="E28" s="13"/>
+    </row>
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B29" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14" t="s">
+    <row r="31" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="14" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="B33" s="0" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
+      <c r="E33" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="2" t="s">
         <v>80</v>
       </c>
     </row>
@@ -924,35 +922,39 @@
         <v>81</v>
       </c>
       <c r="B35" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="E37" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="14" t="s">
         <v>89</v>
       </c>
       <c r="E38" s="0"/>
@@ -961,11 +963,29 @@
       <c r="A39" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="14" t="s">
         <v>92</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>